<commit_message>
Use cluster With STATA 18
</commit_message>
<xml_diff>
--- a/cluster/cluster.xlsx
+++ b/cluster/cluster.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hclust" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -882,7 +884,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1851,4 +1855,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>